<commit_message>
EBITSRL aggiunti files per Accreditamento LDO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34LDO/accreditamento(LDO)-checklist_V8.1.3.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34LDO/accreditamento(LDO)-checklist_V8.1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34LDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96179BE6-A101-49AA-A06B-4D12A61AFEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4487884B-A010-4E3C-96DB-5F303974FC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57465" yWindow="-1725" windowWidth="28875" windowHeight="17280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="-1710" windowWidth="28875" windowHeight="17280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="158">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -719,9 +719,6 @@
     <t>subject_application_version:2.1b34.x</t>
   </si>
   <si>
-    <t>l'ospedalizzazione legata alla BPCO non è gestita dall'applicativo</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a8a52ff8607a2e5ed11b83cb04d452bf3a9ed38d6e681f109347757dd84edfd9.0061e771fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -729,6 +726,18 @@
   </si>
   <si>
     <t>2023-09-20T15:42:36.960Z</t>
+  </si>
+  <si>
+    <t>l'ospedalizzazione legata alla BPCO non viene trattata poiché Suitestensa è utilizzato per le lettere di dimissione in ambito cardiologico</t>
+  </si>
+  <si>
+    <t>2023-09-20T17:23:39.103Z</t>
+  </si>
+  <si>
+    <t>0cb7f69dd5903495</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.f57eaf84fca19f8a37acfbc97d9312c3131f1f1e6c7bdb0fd3955da4cb4bfaa7.3417077500^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3626,10 +3635,10 @@
   <dimension ref="A1:T645"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3900,13 +3909,13 @@
         <v>45189</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>68</v>
@@ -3948,7 +3957,7 @@
         <v>147</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -3978,11 +3987,21 @@
       <c r="E12" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
+      <c r="F12" s="23">
+        <v>45189</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>

</xml_diff>